<commit_message>
4 times the wind power
</commit_message>
<xml_diff>
--- a/group2 project/results/res_bus/p_mw.xlsx
+++ b/group2 project/results/res_bus/p_mw.xlsx
@@ -424,7 +424,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-18.84761551611473</v>
+        <v>98.33082189154038</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>-39.27027815818423</v>
+        <v>-157.0811126327369</v>
       </c>
       <c r="J2">
         <v>-0.09180947066840872</v>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-1.557017206064529</v>
+        <v>117.0706584358068</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>-39.76939137462676</v>
+        <v>-159.0775654985071</v>
       </c>
       <c r="J3">
         <v>-0.09106907171138801</v>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.3586898072596796</v>
+        <v>117.325339161175</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>-39.21276070314079</v>
+        <v>-156.8510428125631</v>
       </c>
       <c r="J4">
         <v>-0.0858862790123851</v>
@@ -574,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.42130931526367</v>
+        <v>115.0606543929562</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>-37.75910917540352</v>
+        <v>-151.0364367016142</v>
       </c>
       <c r="J5">
         <v>-0.08681177770861837</v>
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.489374712105018</v>
+        <v>113.9344408466623</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -645,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>-36.6863929236917</v>
+        <v>-146.7455716947669</v>
       </c>
       <c r="J6">
         <v>-0.0866266779693774</v>
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>15.49025017839676</v>
+        <v>124.9166644827703</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>-36.6863929236917</v>
+        <v>-146.7455716947669</v>
       </c>
       <c r="J7">
         <v>-0.0866266779693774</v>
@@ -724,7 +724,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>18.17790878329038</v>
+        <v>127.0055097470711</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>-36.48649619468827</v>
+        <v>-145.9459847787531</v>
       </c>
       <c r="J8">
         <v>-0.08366508214135138</v>
@@ -774,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>10.3675845361156</v>
+        <v>118.2961956206209</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>-36.17910782839056</v>
+        <v>-144.7164313135622</v>
       </c>
       <c r="J9">
         <v>-0.08403528161986173</v>
@@ -824,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-19.69552273777981</v>
+        <v>91.28743648603427</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>-37.18707765529936</v>
+        <v>-148.7483106211975</v>
       </c>
       <c r="J10">
         <v>-0.0858862790123851</v>
@@ -874,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-52.26237632495349</v>
+        <v>60.87609920852447</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>-37.89080214624073</v>
+        <v>-151.5632085849628</v>
       </c>
       <c r="J11">
         <v>-0.08088858605259475</v>
@@ -924,7 +924,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-63.82773632146177</v>
+        <v>48.41386117890852</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>-37.58184226477783</v>
+        <v>-150.3273690591114</v>
       </c>
       <c r="J12">
         <v>-1.057104610861359</v>
@@ -974,7 +974,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-67.07750751751269</v>
+        <v>44.14817850620693</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -995,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>-37.23736614058328</v>
+        <v>-148.949464562333</v>
       </c>
       <c r="J13">
         <v>-7.595197600678148</v>
@@ -1024,7 +1024,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-63.38963396911004</v>
+        <v>46.35620485809864</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>-36.741710257504</v>
+        <v>-146.9668410300159</v>
       </c>
       <c r="J14">
         <v>-13.42287779125041</v>
@@ -1074,7 +1074,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-59.41941412923393</v>
+        <v>48.12812539728429</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>-36.00561255416113</v>
+        <v>-144.0224502166446</v>
       </c>
       <c r="J15">
         <v>-15.74495402015174</v>
@@ -1124,7 +1124,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-57.86153978682387</v>
+        <v>51.82599569214176</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>-36.72505219675372</v>
+        <v>-146.9002087870148</v>
       </c>
       <c r="J16">
         <v>-16.60696350584271</v>
@@ -1174,7 +1174,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-56.43112285542816</v>
+        <v>56.03530794402536</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>-37.65916081090182</v>
+        <v>-150.6366432436073</v>
       </c>
       <c r="J17">
         <v>-17.25</v>
@@ -1224,7 +1224,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-49.36377664711154</v>
+        <v>62.82017645987594</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1245,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>-37.56895584042388</v>
+        <v>-150.2758233616954</v>
       </c>
       <c r="J18">
         <v>-16.67711630701876</v>
@@ -1274,7 +1274,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-46.18761868785487</v>
+        <v>67.23338340370105</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>-37.98697887434616</v>
+        <v>-151.9479154973845</v>
       </c>
       <c r="J19">
         <v>-14.63768737995343</v>
@@ -1324,7 +1324,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-53.71358902473526</v>
+        <v>59.47376180224251</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>-37.90494578272683</v>
+        <v>-151.6197831309072</v>
       </c>
       <c r="J20">
         <v>-7.235178607835337</v>
@@ -1374,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-72.33047157877172</v>
+        <v>42.2969152050116</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>-38.37765754439528</v>
+        <v>-153.5106301775812</v>
       </c>
       <c r="J21">
         <v>-0.6650633631281266</v>
@@ -1424,7 +1424,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-83.93328975729355</v>
+        <v>33.89216090204673</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>-39.44408773544666</v>
+        <v>-157.7763509417866</v>
       </c>
       <c r="J22">
         <v>-0.1155022372925032</v>
@@ -1474,7 +1474,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-92.04840548889388</v>
+        <v>29.21873965769328</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>-40.59443683631548</v>
+        <v>-162.3777473452619</v>
       </c>
       <c r="J23">
         <v>-0.1084684472009485</v>
@@ -1524,7 +1524,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-94.68488722073516</v>
+        <v>28.99733288624952</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>-41.40376714635295</v>
+        <v>-165.6150685854118</v>
       </c>
       <c r="J24">
         <v>-0.1012495573701813</v>
@@ -1574,7 +1574,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-76.08070572768224</v>
+        <v>49.33643119517637</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1595,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>-42</v>
+        <v>-168</v>
       </c>
       <c r="J25">
         <v>-0.09884326075990657</v>

</xml_diff>